<commit_message>
Mudança no coeficiente de P
</commit_message>
<xml_diff>
--- a/March2024/Results/Only_Yearly/Results_Stats.xlsx
+++ b/March2024/Results/Only_Yearly/Results_Stats.xlsx
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>100.0</v>
+        <v>97.64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>95.91</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -511,7 +511,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>93.67</v>
+        <v>93.37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>93.37</v>
+        <v>93.33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -527,7 +527,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>93.37</v>
+        <v>93.33</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -551,7 +551,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>91.13</v>
+        <v>89.56</v>
       </c>
     </row>
   </sheetData>
@@ -604,352 +604,352 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>85.44336947794616</v>
+        <v>81.93936947794616</v>
       </c>
       <c r="B2">
-        <v>76.95896719657495</v>
+        <v>73.45496719657494</v>
       </c>
       <c r="C2">
-        <v>74.96514056540812</v>
+        <v>71.46114056540813</v>
       </c>
       <c r="D2">
-        <v>80.07231891577662</v>
+        <v>76.56831891577663</v>
       </c>
       <c r="E2">
-        <v>82.00707698478536</v>
+        <v>78.50307698478537</v>
       </c>
       <c r="F2">
-        <v>84.08278795051626</v>
+        <v>80.57878795051627</v>
       </c>
       <c r="G2">
-        <v>85.52286235588173</v>
+        <v>82.01886235588172</v>
       </c>
       <c r="H2">
-        <v>87.00293334848615</v>
+        <v>83.49893334848616</v>
       </c>
       <c r="I2">
-        <v>88.74238890122473</v>
+        <v>85.23838890122474</v>
       </c>
       <c r="J2">
-        <v>90.24703483638199</v>
+        <v>86.74303483638201</v>
       </c>
       <c r="K2">
-        <v>95.39370435195002</v>
+        <v>91.88970435195002</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>85.44336947794616</v>
+        <v>81.93936947794616</v>
       </c>
       <c r="B3">
-        <v>76.95896719657495</v>
+        <v>73.45496719657494</v>
       </c>
       <c r="C3">
-        <v>74.96514056540812</v>
+        <v>71.46114056540813</v>
       </c>
       <c r="D3">
-        <v>80.07231891577662</v>
+        <v>76.56831891577663</v>
       </c>
       <c r="E3">
-        <v>82.00707698478536</v>
+        <v>78.50307698478537</v>
       </c>
       <c r="F3">
-        <v>84.08278795051626</v>
+        <v>80.57878795051627</v>
       </c>
       <c r="G3">
-        <v>85.52286235588173</v>
+        <v>82.01886235588172</v>
       </c>
       <c r="H3">
-        <v>87.00293334848615</v>
+        <v>83.49893334848616</v>
       </c>
       <c r="I3">
-        <v>88.74238890122473</v>
+        <v>85.23838890122474</v>
       </c>
       <c r="J3">
-        <v>90.24703483638199</v>
+        <v>86.74303483638201</v>
       </c>
       <c r="K3">
-        <v>95.39370435195002</v>
+        <v>91.88970435195002</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>85.44336947794616</v>
+        <v>81.83194065223961</v>
       </c>
       <c r="B4">
-        <v>76.95896719657495</v>
+        <v>74.74535188773635</v>
       </c>
       <c r="C4">
-        <v>74.96514056540812</v>
+        <v>72.88202405734792</v>
       </c>
       <c r="D4">
-        <v>80.07231891577662</v>
+        <v>77.27524520582892</v>
       </c>
       <c r="E4">
-        <v>82.00707698478536</v>
+        <v>78.62869189895402</v>
       </c>
       <c r="F4">
-        <v>84.08278795051626</v>
+        <v>80.16143279691184</v>
       </c>
       <c r="G4">
-        <v>85.52286235588173</v>
+        <v>81.52676427473973</v>
       </c>
       <c r="H4">
-        <v>87.00293334848615</v>
+        <v>83.0283825776067</v>
       </c>
       <c r="I4">
-        <v>88.74238890122473</v>
+        <v>85.07037489744788</v>
       </c>
       <c r="J4">
-        <v>90.24703483638199</v>
+        <v>87.84418794740816</v>
       </c>
       <c r="K4">
-        <v>95.39370435195002</v>
+        <v>94.09990444760692</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>85.11429798462026</v>
+        <v>81.65528076353313</v>
       </c>
       <c r="B5">
-        <v>78.70002989328214</v>
+        <v>75.78554483863378</v>
       </c>
       <c r="C5">
-        <v>77.25363629393377</v>
+        <v>74.78243767904854</v>
       </c>
       <c r="D5">
-        <v>80.9052156141313</v>
+        <v>77.40078808070729</v>
       </c>
       <c r="E5">
-        <v>81.77638945539559</v>
+        <v>78.10066444499289</v>
       </c>
       <c r="F5">
-        <v>83.18289196018554</v>
+        <v>79.29567576097303</v>
       </c>
       <c r="G5">
-        <v>84.45288072354984</v>
+        <v>80.56187224731259</v>
       </c>
       <c r="H5">
-        <v>86.22891128376104</v>
+        <v>82.50939666541798</v>
       </c>
       <c r="I5">
-        <v>88.73612166030705</v>
+        <v>86.12790627262274</v>
       </c>
       <c r="J5">
-        <v>91.90078876253988</v>
+        <v>90.81349408987724</v>
       </c>
       <c r="K5">
-        <v>99.38664969967746</v>
+        <v>99.14248434247484</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>84.93421615193097</v>
+        <v>81.63821313664103</v>
       </c>
       <c r="B6">
-        <v>79.07708296554718</v>
+        <v>75.82167835099672</v>
       </c>
       <c r="C6">
-        <v>78.05434423895208</v>
+        <v>74.73038858488631</v>
       </c>
       <c r="D6">
-        <v>80.6703093695088</v>
+        <v>77.33394100779675</v>
       </c>
       <c r="E6">
-        <v>81.36964922093343</v>
+        <v>78.00362865271136</v>
       </c>
       <c r="F6">
-        <v>82.55900383868172</v>
+        <v>79.20419001685895</v>
       </c>
       <c r="G6">
-        <v>83.83955147009483</v>
+        <v>80.49197263998364</v>
       </c>
       <c r="H6">
-        <v>85.78700497580137</v>
+        <v>82.47372967994528</v>
       </c>
       <c r="I6">
-        <v>89.39341229113913</v>
+        <v>86.17155893759588</v>
       </c>
       <c r="J6">
-        <v>94.14055116217357</v>
+        <v>91.05119266903736</v>
       </c>
       <c r="K6">
-        <v>102.54735520397527</v>
+        <v>99.75217943060038</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>84.91006480784282</v>
+        <v>81.63618631913042</v>
       </c>
       <c r="B7">
-        <v>79.09353002219851</v>
+        <v>75.82348488166237</v>
       </c>
       <c r="C7">
-        <v>78.00224025608809</v>
+        <v>74.7242076426776</v>
       </c>
       <c r="D7">
-        <v>80.60579267899853</v>
+        <v>77.33964343972544</v>
       </c>
       <c r="E7">
-        <v>81.27548032391313</v>
+        <v>77.9886129556204</v>
       </c>
       <c r="F7">
-        <v>82.47604168806073</v>
+        <v>79.19492661693559</v>
       </c>
       <c r="G7">
-        <v>83.76382431118542</v>
+        <v>80.48687982127764</v>
       </c>
       <c r="H7">
-        <v>85.74558135114704</v>
+        <v>82.48596428461953</v>
       </c>
       <c r="I7">
-        <v>89.44341060879763</v>
+        <v>86.18741869982271</v>
       </c>
       <c r="J7">
-        <v>94.32304434023914</v>
+        <v>91.12221978814586</v>
       </c>
       <c r="K7">
-        <v>103.02403110180212</v>
+        <v>99.82458203750988</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>84.91006480784282</v>
+        <v>81.63618631913042</v>
       </c>
       <c r="B8">
-        <v>79.09353002219851</v>
+        <v>75.82348488166237</v>
       </c>
       <c r="C8">
-        <v>78.00224025608809</v>
+        <v>74.7242076426776</v>
       </c>
       <c r="D8">
-        <v>80.60579267899853</v>
+        <v>77.33964343972544</v>
       </c>
       <c r="E8">
-        <v>81.27548032391313</v>
+        <v>77.9886129556204</v>
       </c>
       <c r="F8">
-        <v>82.47604168806073</v>
+        <v>79.19492661693559</v>
       </c>
       <c r="G8">
-        <v>83.76382431118542</v>
+        <v>80.48687982127764</v>
       </c>
       <c r="H8">
-        <v>85.74558135114704</v>
+        <v>82.48596428461953</v>
       </c>
       <c r="I8">
-        <v>89.44341060879763</v>
+        <v>86.18741869982271</v>
       </c>
       <c r="J8">
-        <v>94.32304434023914</v>
+        <v>91.12221978814586</v>
       </c>
       <c r="K8">
-        <v>103.02403110180212</v>
+        <v>99.82458203750988</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>84.90647560484223</v>
+        <v>81.63618631913042</v>
       </c>
       <c r="B9">
-        <v>79.09377416737418</v>
+        <v>75.82348488166237</v>
       </c>
       <c r="C9">
-        <v>77.99449692838942</v>
+        <v>74.7242076426776</v>
       </c>
       <c r="D9">
-        <v>80.60993272543725</v>
+        <v>77.33964343972544</v>
       </c>
       <c r="E9">
-        <v>81.25890224133222</v>
+        <v>77.9886129556204</v>
       </c>
       <c r="F9">
-        <v>82.4652159026474</v>
+        <v>79.19492661693559</v>
       </c>
       <c r="G9">
-        <v>83.75716910698944</v>
+        <v>80.48687982127764</v>
       </c>
       <c r="H9">
-        <v>85.75625357033135</v>
+        <v>82.48596428461953</v>
       </c>
       <c r="I9">
-        <v>89.45770798553451</v>
+        <v>86.18741869982271</v>
       </c>
       <c r="J9">
-        <v>94.39250907385767</v>
+        <v>91.12221978814586</v>
       </c>
       <c r="K9">
-        <v>103.09487132322171</v>
+        <v>99.82458203750988</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>84.90647560484223</v>
+        <v>81.63618631913042</v>
       </c>
       <c r="B10">
-        <v>79.09377416737418</v>
+        <v>75.82348488166237</v>
       </c>
       <c r="C10">
-        <v>77.99449692838942</v>
+        <v>74.7242076426776</v>
       </c>
       <c r="D10">
-        <v>80.60993272543725</v>
+        <v>77.33964343972544</v>
       </c>
       <c r="E10">
-        <v>81.25890224133222</v>
+        <v>77.9886129556204</v>
       </c>
       <c r="F10">
-        <v>82.4652159026474</v>
+        <v>79.19492661693559</v>
       </c>
       <c r="G10">
-        <v>83.75716910698944</v>
+        <v>80.48687982127764</v>
       </c>
       <c r="H10">
-        <v>85.75625357033135</v>
+        <v>82.48596428461953</v>
       </c>
       <c r="I10">
-        <v>89.45770798553451</v>
+        <v>86.18741869982271</v>
       </c>
       <c r="J10">
-        <v>94.39250907385767</v>
+        <v>91.12221978814586</v>
       </c>
       <c r="K10">
-        <v>103.09487132322171</v>
+        <v>99.82458203750988</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>84.72908359845424</v>
+        <v>81.46465583119641</v>
       </c>
       <c r="B11">
-        <v>78.88370307232803</v>
+        <v>75.5089449774794</v>
       </c>
       <c r="C11">
-        <v>78.15615385639175</v>
+        <v>74.98897253472948</v>
       </c>
       <c r="D11">
-        <v>80.05456834478497</v>
+        <v>76.49997115894458</v>
       </c>
       <c r="E11">
-        <v>80.76561428876755</v>
+        <v>77.18105468021393</v>
       </c>
       <c r="F11">
-        <v>81.86992705787624</v>
+        <v>78.28970801900307</v>
       </c>
       <c r="G11">
-        <v>83.24073739325358</v>
+        <v>79.63355254679018</v>
       </c>
       <c r="H11">
-        <v>85.33810573241985</v>
+        <v>82.02601548596317</v>
       </c>
       <c r="I11">
-        <v>90.20206397801465</v>
+        <v>87.69665586835072</v>
       </c>
       <c r="J11">
-        <v>96.24616964351813</v>
+        <v>94.50774743486019</v>
       </c>
       <c r="K11">
-        <v>107.03443659435769</v>
+        <v>106.53725810095804</v>
       </c>
     </row>
   </sheetData>
@@ -1002,352 +1002,352 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>85.49590297005693</v>
+        <v>81.99190297005694</v>
       </c>
       <c r="B2">
-        <v>77.55317604564028</v>
+        <v>74.0491760456403</v>
       </c>
       <c r="C2">
-        <v>75.88072751229083</v>
+        <v>72.37672751229083</v>
       </c>
       <c r="D2">
-        <v>80.25570523180325</v>
+        <v>76.75170523180327</v>
       </c>
       <c r="E2">
-        <v>81.93204310247208</v>
+        <v>78.42804310247209</v>
       </c>
       <c r="F2">
-        <v>83.95423469847036</v>
+        <v>80.45023469847035</v>
       </c>
       <c r="G2">
-        <v>85.56508680795898</v>
+        <v>82.06108680795897</v>
       </c>
       <c r="H2">
-        <v>86.97010486422707</v>
+        <v>83.46610486422708</v>
       </c>
       <c r="I2">
-        <v>88.62907615229177</v>
+        <v>85.12507615229177</v>
       </c>
       <c r="J2">
-        <v>89.95494560446284</v>
+        <v>86.45094560446282</v>
       </c>
       <c r="K2">
-        <v>97.4759943686047</v>
+        <v>93.97199436860471</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>85.49590297005693</v>
+        <v>81.99190297005694</v>
       </c>
       <c r="B3">
-        <v>77.55317604564028</v>
+        <v>74.0491760456403</v>
       </c>
       <c r="C3">
-        <v>75.88072751229083</v>
+        <v>72.37672751229083</v>
       </c>
       <c r="D3">
-        <v>80.25570523180325</v>
+        <v>76.75170523180327</v>
       </c>
       <c r="E3">
-        <v>81.93204310247208</v>
+        <v>78.42804310247209</v>
       </c>
       <c r="F3">
-        <v>83.95423469847036</v>
+        <v>80.45023469847035</v>
       </c>
       <c r="G3">
-        <v>85.56508680795898</v>
+        <v>82.06108680795897</v>
       </c>
       <c r="H3">
-        <v>86.97010486422707</v>
+        <v>83.46610486422708</v>
       </c>
       <c r="I3">
-        <v>88.62907615229177</v>
+        <v>85.12507615229177</v>
       </c>
       <c r="J3">
-        <v>89.95494560446284</v>
+        <v>86.45094560446282</v>
       </c>
       <c r="K3">
-        <v>97.4759943686047</v>
+        <v>93.97199436860471</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>85.49590297005693</v>
+        <v>81.86553135906756</v>
       </c>
       <c r="B4">
-        <v>77.55317604564028</v>
+        <v>75.08005066876817</v>
       </c>
       <c r="C4">
-        <v>75.88072751229083</v>
+        <v>73.13697853605835</v>
       </c>
       <c r="D4">
-        <v>80.25570523180325</v>
+        <v>77.23151682911471</v>
       </c>
       <c r="E4">
-        <v>81.93204310247208</v>
+        <v>78.42588711828934</v>
       </c>
       <c r="F4">
-        <v>83.95423469847036</v>
+        <v>80.07235649461062</v>
       </c>
       <c r="G4">
-        <v>85.56508680795898</v>
+        <v>81.54466296777733</v>
       </c>
       <c r="H4">
-        <v>86.97010486422707</v>
+        <v>83.09820299571483</v>
       </c>
       <c r="I4">
-        <v>88.62907615229177</v>
+        <v>85.0262743517023</v>
       </c>
       <c r="J4">
-        <v>89.95494560446284</v>
+        <v>87.38898997181445</v>
       </c>
       <c r="K4">
-        <v>97.4759943686047</v>
+        <v>96.74363932462612</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>85.13406498868747</v>
+        <v>81.65772126167327</v>
       </c>
       <c r="B5">
-        <v>78.9867597786471</v>
+        <v>75.9343997108673</v>
       </c>
       <c r="C5">
-        <v>77.18579981069551</v>
+        <v>74.61925652705791</v>
       </c>
       <c r="D5">
-        <v>80.4752340102161</v>
+        <v>77.26346633272786</v>
       </c>
       <c r="E5">
-        <v>81.71823818582618</v>
+        <v>78.02399578663815</v>
       </c>
       <c r="F5">
-        <v>83.11931280338774</v>
+        <v>79.37892144894387</v>
       </c>
       <c r="G5">
-        <v>84.57045094417947</v>
+        <v>80.81105224064686</v>
       </c>
       <c r="H5">
-        <v>86.15087900265175</v>
+        <v>82.44708139808967</v>
       </c>
       <c r="I5">
-        <v>88.42784759626507</v>
+        <v>85.24545873200816</v>
       </c>
       <c r="J5">
-        <v>91.71851962391156</v>
+        <v>89.73781589444846</v>
       </c>
       <c r="K5">
-        <v>102.12703193723827</v>
+        <v>100.83691246599874</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>84.93605194853305</v>
+        <v>81.63764412230279</v>
       </c>
       <c r="B6">
-        <v>79.21819223812948</v>
+        <v>75.9361794889809</v>
       </c>
       <c r="C6">
-        <v>77.89758900183892</v>
+        <v>74.59918828591381</v>
       </c>
       <c r="D6">
-        <v>80.54757994853027</v>
+        <v>77.20373929887188</v>
       </c>
       <c r="E6">
-        <v>81.29479640188164</v>
+        <v>77.9487532121571</v>
       </c>
       <c r="F6">
-        <v>82.654750944962</v>
+        <v>79.34419794933474</v>
       </c>
       <c r="G6">
-        <v>84.07881928993156</v>
+        <v>80.72412042579957</v>
       </c>
       <c r="H6">
-        <v>85.71747385954083</v>
+        <v>82.43229111972138</v>
       </c>
       <c r="I6">
-        <v>88.53041421888325</v>
+        <v>85.2583522683476</v>
       </c>
       <c r="J6">
-        <v>93.03082518908391</v>
+        <v>89.79079207226889</v>
       </c>
       <c r="K6">
-        <v>104.189797427717</v>
+        <v>101.18788121683912</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>84.90949579350455</v>
+        <v>81.63525991869342</v>
       </c>
       <c r="B7">
-        <v>79.20803116018268</v>
+        <v>75.93524385306277</v>
       </c>
       <c r="C7">
-        <v>77.8710399571156</v>
+        <v>74.59680513898803</v>
       </c>
       <c r="D7">
-        <v>80.47559097007365</v>
+        <v>77.19401877233565</v>
       </c>
       <c r="E7">
-        <v>81.2206048833589</v>
+        <v>77.93749362957232</v>
       </c>
       <c r="F7">
-        <v>82.61604962053653</v>
+        <v>79.3318882821361</v>
       </c>
       <c r="G7">
-        <v>83.99597209700134</v>
+        <v>80.70910472870861</v>
       </c>
       <c r="H7">
-        <v>85.70414279092316</v>
+        <v>82.42108047564709</v>
       </c>
       <c r="I7">
-        <v>88.53020393954938</v>
+        <v>85.25988340360101</v>
       </c>
       <c r="J7">
-        <v>93.06264374347067</v>
+        <v>89.79708310766182</v>
       </c>
       <c r="K7">
-        <v>104.45973288804092</v>
+        <v>101.22955951308842</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>84.90949579350455</v>
+        <v>81.63525991869342</v>
       </c>
       <c r="B8">
-        <v>79.20803116018268</v>
+        <v>75.93524385306277</v>
       </c>
       <c r="C8">
-        <v>77.8710399571156</v>
+        <v>74.59680513898803</v>
       </c>
       <c r="D8">
-        <v>80.47559097007365</v>
+        <v>77.19401877233565</v>
       </c>
       <c r="E8">
-        <v>81.2206048833589</v>
+        <v>77.93749362957232</v>
       </c>
       <c r="F8">
-        <v>82.61604962053653</v>
+        <v>79.3318882821361</v>
       </c>
       <c r="G8">
-        <v>83.99597209700134</v>
+        <v>80.70910472870861</v>
       </c>
       <c r="H8">
-        <v>85.70414279092316</v>
+        <v>82.42108047564709</v>
       </c>
       <c r="I8">
-        <v>88.53020393954938</v>
+        <v>85.25988340360101</v>
       </c>
       <c r="J8">
-        <v>93.06264374347067</v>
+        <v>89.79708310766182</v>
       </c>
       <c r="K8">
-        <v>104.45973288804092</v>
+        <v>101.22955951308842</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>84.90554920440525</v>
+        <v>81.63525991869342</v>
       </c>
       <c r="B9">
-        <v>79.20553313877458</v>
+        <v>75.93524385306277</v>
       </c>
       <c r="C9">
-        <v>77.86709442469987</v>
+        <v>74.59680513898803</v>
       </c>
       <c r="D9">
-        <v>80.46430805804748</v>
+        <v>77.19401877233565</v>
       </c>
       <c r="E9">
-        <v>81.20778291528416</v>
+        <v>77.93749362957232</v>
       </c>
       <c r="F9">
-        <v>82.60217756784793</v>
+        <v>79.3318882821361</v>
       </c>
       <c r="G9">
-        <v>83.97939401442042</v>
+        <v>80.70910472870861</v>
       </c>
       <c r="H9">
-        <v>85.69136976135891</v>
+        <v>82.42108047564709</v>
       </c>
       <c r="I9">
-        <v>88.53017268931282</v>
+        <v>85.25988340360101</v>
       </c>
       <c r="J9">
-        <v>93.06737239337367</v>
+        <v>89.79708310766182</v>
       </c>
       <c r="K9">
-        <v>104.49984879880023</v>
+        <v>101.22955951308842</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>84.90554920440525</v>
+        <v>81.63525991869342</v>
       </c>
       <c r="B10">
-        <v>79.20553313877458</v>
+        <v>75.93524385306277</v>
       </c>
       <c r="C10">
-        <v>77.86709442469987</v>
+        <v>74.59680513898803</v>
       </c>
       <c r="D10">
-        <v>80.46430805804748</v>
+        <v>77.19401877233565</v>
       </c>
       <c r="E10">
-        <v>81.20778291528416</v>
+        <v>77.93749362957232</v>
       </c>
       <c r="F10">
-        <v>82.60217756784793</v>
+        <v>79.3318882821361</v>
       </c>
       <c r="G10">
-        <v>83.97939401442042</v>
+        <v>80.70910472870861</v>
       </c>
       <c r="H10">
-        <v>85.69136976135891</v>
+        <v>82.42108047564709</v>
       </c>
       <c r="I10">
-        <v>88.53017268931282</v>
+        <v>85.25988340360101</v>
       </c>
       <c r="J10">
-        <v>93.06737239337367</v>
+        <v>89.79708310766182</v>
       </c>
       <c r="K10">
-        <v>104.49984879880023</v>
+        <v>101.22955951308842</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>84.71049382341866</v>
+        <v>81.4334836826465</v>
       </c>
       <c r="B11">
-        <v>79.01300934744226</v>
+        <v>75.65215050072545</v>
       </c>
       <c r="C11">
-        <v>78.1784455449543</v>
+        <v>75.20577313119506</v>
       </c>
       <c r="D11">
-        <v>80.02183682534125</v>
+        <v>76.48545647436838</v>
       </c>
       <c r="E11">
-        <v>80.69674926187237</v>
+        <v>77.19304281051501</v>
       </c>
       <c r="F11">
-        <v>81.92634331318723</v>
+        <v>78.36790803994197</v>
       </c>
       <c r="G11">
-        <v>83.35163849054143</v>
+        <v>79.78670226774847</v>
       </c>
       <c r="H11">
-        <v>85.22377884117829</v>
+        <v>82.02825435680636</v>
       </c>
       <c r="I11">
-        <v>89.08922282918613</v>
+        <v>86.39482739713175</v>
       </c>
       <c r="J11">
-        <v>93.88417933232003</v>
+        <v>91.68747430285129</v>
       </c>
       <c r="K11">
-        <v>108.23852746115294</v>
+        <v>108.00401266013469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>